<commit_message>
recreate all xlsx files after merging multiple branches to get correct supplementary numbers
</commit_message>
<xml_diff>
--- a/manuscript/tables/S1_datasets.xlsx
+++ b/manuscript/tables/S1_datasets.xlsx
@@ -726,7 +726,7 @@
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4706,7 +4706,7 @@
         <v>6517</v>
       </c>
       <c r="F14" t="n">
-        <v>3644.9500637398</v>
+        <v>3644.95006373981</v>
       </c>
       <c r="G14" t="s">
         <v>97</v>
@@ -5174,7 +5174,7 @@
         <v>6517</v>
       </c>
       <c r="F32" t="n">
-        <v>3644.9500637398</v>
+        <v>3644.95006373981</v>
       </c>
       <c r="G32" t="s">
         <v>97</v>
@@ -5642,7 +5642,7 @@
         <v>6517</v>
       </c>
       <c r="F50" t="n">
-        <v>3644.9500637398</v>
+        <v>3644.95006373981</v>
       </c>
       <c r="G50" t="s">
         <v>97</v>

</xml_diff>

<commit_message>
datasets supplementary table: summarize total sample sizes for mrmega analyses
</commit_message>
<xml_diff>
--- a/manuscript/tables/S1_datasets.xlsx
+++ b/manuscript/tables/S1_datasets.xlsx
@@ -4706,7 +4706,7 @@
         <v>6517</v>
       </c>
       <c r="F14" t="n">
-        <v>3644.95006373981</v>
+        <v>3644.9500637398</v>
       </c>
       <c r="G14" t="s">
         <v>97</v>
@@ -5174,7 +5174,7 @@
         <v>6517</v>
       </c>
       <c r="F32" t="n">
-        <v>3644.95006373981</v>
+        <v>3644.9500637398</v>
       </c>
       <c r="G32" t="s">
         <v>97</v>
@@ -5194,13 +5194,13 @@
         <v>112</v>
       </c>
       <c r="D33" t="n">
-        <v>14021</v>
+        <v>241923</v>
       </c>
       <c r="E33" t="n">
-        <v>34482</v>
+        <v>578645</v>
       </c>
       <c r="F33" t="n">
-        <v>39865.8798186363</v>
+        <v>571649.261518054</v>
       </c>
       <c r="G33" t="s">
         <v>97</v>
@@ -5214,25 +5214,25 @@
         <v>111</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C34" t="s">
         <v>112</v>
       </c>
       <c r="D34" t="n">
-        <v>8351</v>
+        <v>59080</v>
       </c>
       <c r="E34" t="n">
-        <v>28099</v>
+        <v>384869</v>
       </c>
       <c r="F34" t="n">
-        <v>25748.9221695844</v>
+        <v>200410.540548726</v>
       </c>
       <c r="G34" t="s">
         <v>97</v>
       </c>
       <c r="H34" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35">
@@ -5240,414 +5240,24 @@
         <v>111</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="C35" t="s">
         <v>112</v>
       </c>
       <c r="D35" t="n">
-        <v>4091</v>
+        <v>80934</v>
       </c>
       <c r="E35" t="n">
-        <v>179842</v>
+        <v>363887</v>
       </c>
       <c r="F35" t="n">
-        <v>15624.6368147062</v>
+        <v>261413.968732726</v>
       </c>
       <c r="G35" t="s">
         <v>97</v>
       </c>
       <c r="H35" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>111</v>
-      </c>
-      <c r="B36" t="s">
-        <v>40</v>
-      </c>
-      <c r="C36" t="s">
-        <v>112</v>
-      </c>
-      <c r="D36" t="n">
-        <v>213129</v>
-      </c>
-      <c r="E36" t="n">
-        <v>329556</v>
-      </c>
-      <c r="F36" t="n">
-        <v>483572.556026851</v>
-      </c>
-      <c r="G36" t="s">
-        <v>97</v>
-      </c>
-      <c r="H36" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s">
-        <v>111</v>
-      </c>
-      <c r="B37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" t="s">
-        <v>112</v>
-      </c>
-      <c r="D37" t="n">
-        <v>340</v>
-      </c>
-      <c r="E37" t="n">
-        <v>1069</v>
-      </c>
-      <c r="F37" t="n">
-        <v>1023.26056018038</v>
-      </c>
-      <c r="G37" t="s">
-        <v>97</v>
-      </c>
-      <c r="H37" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s">
-        <v>111</v>
-      </c>
-      <c r="B38" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" t="s">
-        <v>112</v>
-      </c>
-      <c r="D38" t="n">
-        <v>1991</v>
-      </c>
-      <c r="E38" t="n">
-        <v>5597</v>
-      </c>
-      <c r="F38" t="n">
-        <v>5814.00612809532</v>
-      </c>
-      <c r="G38" t="s">
-        <v>97</v>
-      </c>
-      <c r="H38" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s">
-        <v>111</v>
-      </c>
-      <c r="B39" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" t="s">
-        <v>112</v>
-      </c>
-      <c r="D39" t="n">
-        <v>4227</v>
-      </c>
-      <c r="E39" t="n">
-        <v>44277</v>
-      </c>
-      <c r="F39" t="n">
-        <v>15310.3275655298</v>
-      </c>
-      <c r="G39" t="s">
-        <v>97</v>
-      </c>
-      <c r="H39" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s">
-        <v>111</v>
-      </c>
-      <c r="B40" t="s">
-        <v>55</v>
-      </c>
-      <c r="C40" t="s">
-        <v>112</v>
-      </c>
-      <c r="D40" t="n">
-        <v>2305</v>
-      </c>
-      <c r="E40" t="n">
-        <v>33847</v>
-      </c>
-      <c r="F40" t="n">
-        <v>8632.14593936712</v>
-      </c>
-      <c r="G40" t="s">
-        <v>97</v>
-      </c>
-      <c r="H40" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s">
-        <v>111</v>
-      </c>
-      <c r="B41" t="s">
-        <v>55</v>
-      </c>
-      <c r="C41" t="s">
-        <v>112</v>
-      </c>
-      <c r="D41" t="n">
-        <v>140</v>
-      </c>
-      <c r="E41" t="n">
-        <v>4086</v>
-      </c>
-      <c r="F41" t="n">
-        <v>541.448177946048</v>
-      </c>
-      <c r="G41" t="s">
-        <v>97</v>
-      </c>
-      <c r="H41" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s">
-        <v>111</v>
-      </c>
-      <c r="B42" t="s">
-        <v>55</v>
-      </c>
-      <c r="C42" t="s">
-        <v>112</v>
-      </c>
-      <c r="D42" t="n">
-        <v>51117</v>
-      </c>
-      <c r="E42" t="n">
-        <v>295841</v>
-      </c>
-      <c r="F42" t="n">
-        <v>171785.756394887</v>
-      </c>
-      <c r="G42" t="s">
-        <v>97</v>
-      </c>
-      <c r="H42" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s">
-        <v>111</v>
-      </c>
-      <c r="B43" t="s">
-        <v>55</v>
-      </c>
-      <c r="C43" t="s">
-        <v>112</v>
-      </c>
-      <c r="D43" t="n">
-        <v>113</v>
-      </c>
-      <c r="E43" t="n">
-        <v>419</v>
-      </c>
-      <c r="F43" t="n">
-        <v>355.992481203008</v>
-      </c>
-      <c r="G43" t="s">
-        <v>97</v>
-      </c>
-      <c r="H43" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s">
-        <v>111</v>
-      </c>
-      <c r="B44" t="s">
-        <v>55</v>
-      </c>
-      <c r="C44" t="s">
-        <v>112</v>
-      </c>
-      <c r="D44" t="n">
-        <v>1178</v>
-      </c>
-      <c r="E44" t="n">
-        <v>6399</v>
-      </c>
-      <c r="F44" t="n">
-        <v>3784.86998979291</v>
-      </c>
-      <c r="G44" t="s">
-        <v>97</v>
-      </c>
-      <c r="H44" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s">
-        <v>111</v>
-      </c>
-      <c r="B45" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" t="s">
-        <v>112</v>
-      </c>
-      <c r="D45" t="n">
-        <v>8276</v>
-      </c>
-      <c r="E45" t="n">
-        <v>40228</v>
-      </c>
-      <c r="F45" t="n">
-        <v>27437.1429778177</v>
-      </c>
-      <c r="G45" t="s">
-        <v>97</v>
-      </c>
-      <c r="H45" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s">
-        <v>111</v>
-      </c>
-      <c r="B46" t="s">
-        <v>61</v>
-      </c>
-      <c r="C46" t="s">
-        <v>112</v>
-      </c>
-      <c r="D46" t="n">
-        <v>5203</v>
-      </c>
-      <c r="E46" t="n">
-        <v>30949</v>
-      </c>
-      <c r="F46" t="n">
-        <v>17816.7345651693</v>
-      </c>
-      <c r="G46" t="s">
-        <v>97</v>
-      </c>
-      <c r="H46" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s">
-        <v>111</v>
-      </c>
-      <c r="B47" t="s">
-        <v>61</v>
-      </c>
-      <c r="C47" t="s">
-        <v>112</v>
-      </c>
-      <c r="D47" t="n">
-        <v>431</v>
-      </c>
-      <c r="E47" t="n">
-        <v>3795</v>
-      </c>
-      <c r="F47" t="n">
-        <v>1548.17321344061</v>
-      </c>
-      <c r="G47" t="s">
-        <v>97</v>
-      </c>
-      <c r="H47" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s">
-        <v>111</v>
-      </c>
-      <c r="B48" t="s">
-        <v>61</v>
-      </c>
-      <c r="C48" t="s">
-        <v>112</v>
-      </c>
-      <c r="D48" t="n">
-        <v>65762</v>
-      </c>
-      <c r="E48" t="n">
-        <v>281196</v>
-      </c>
-      <c r="F48" t="n">
-        <v>210276.808155368</v>
-      </c>
-      <c r="G48" t="s">
-        <v>97</v>
-      </c>
-      <c r="H48" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s">
-        <v>111</v>
-      </c>
-      <c r="B49" t="s">
-        <v>61</v>
-      </c>
-      <c r="C49" t="s">
-        <v>112</v>
-      </c>
-      <c r="D49" t="n">
-        <v>202</v>
-      </c>
-      <c r="E49" t="n">
-        <v>1202</v>
-      </c>
-      <c r="F49" t="n">
-        <v>690.159757191143</v>
-      </c>
-      <c r="G49" t="s">
-        <v>97</v>
-      </c>
-      <c r="H49" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s">
-        <v>111</v>
-      </c>
-      <c r="B50" t="s">
-        <v>61</v>
-      </c>
-      <c r="C50" t="s">
-        <v>112</v>
-      </c>
-      <c r="D50" t="n">
-        <v>1060</v>
-      </c>
-      <c r="E50" t="n">
-        <v>6517</v>
-      </c>
-      <c r="F50" t="n">
-        <v>3644.95006373981</v>
-      </c>
-      <c r="G50" t="s">
-        <v>97</v>
-      </c>
-      <c r="H50" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>

<commit_message>
move clump/finemapping and popcorn results for online vs supplementary materials
</commit_message>
<xml_diff>
--- a/manuscript/tables/S1_datasets.xlsx
+++ b/manuscript/tables/S1_datasets.xlsx
@@ -4706,7 +4706,7 @@
         <v>6517</v>
       </c>
       <c r="F14" t="n">
-        <v>3644.95006373981</v>
+        <v>3644.9500637398</v>
       </c>
       <c r="G14" t="s">
         <v>97</v>
@@ -5174,7 +5174,7 @@
         <v>6517</v>
       </c>
       <c r="F32" t="n">
-        <v>3644.95006373981</v>
+        <v>3644.9500637398</v>
       </c>
       <c r="G32" t="s">
         <v>97</v>

</xml_diff>